<commit_message>
Add `flask_name` attribute to reagents.
</commit_message>
<xml_diff>
--- a/sample_data/data.xlsx
+++ b/sample_data/data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uigedail\Code\chem_oracle\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B98F63B4-D96A-4B87-9CB3-5F178063821B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1225F259-B2CB-42E1-AF97-6A52BB16DCB5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="5715" yWindow="3405" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="reagents" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
   <si>
     <t>compound1</t>
   </si>
@@ -210,12 +210,15 @@
   </si>
   <si>
     <t>CN(C)P(Cl)Cl</t>
+  </si>
+  <si>
+    <t>flask_name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1049,11 +1052,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,11 +1064,12 @@
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1"/>
+    <col min="5" max="5" width="72.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1076,13 +1080,16 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1093,10 +1100,13 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1107,10 +1117,13 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1121,10 +1134,13 @@
         <v>21</v>
       </c>
       <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1135,10 +1151,13 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1149,10 +1168,13 @@
         <v>27</v>
       </c>
       <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1163,10 +1185,13 @@
         <v>31</v>
       </c>
       <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1177,10 +1202,13 @@
         <v>34</v>
       </c>
       <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1191,10 +1219,13 @@
         <v>37</v>
       </c>
       <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1205,10 +1236,13 @@
         <v>40</v>
       </c>
       <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1219,10 +1253,13 @@
         <v>43</v>
       </c>
       <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1233,10 +1270,13 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1247,10 +1287,13 @@
         <v>49</v>
       </c>
       <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1261,10 +1304,13 @@
         <v>52</v>
       </c>
       <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1275,10 +1321,13 @@
         <v>54</v>
       </c>
       <c r="D15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1289,10 +1338,13 @@
         <v>57</v>
       </c>
       <c r="D16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1303,6 +1355,9 @@
         <v>60</v>
       </c>
       <c r="D17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1312,11 +1367,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>